<commit_message>
se realizan cambios para sanity en semilla 9, se hace ajuste de tiempos y mapeo
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/dataReno-Repo.xlsx
+++ b/src/test/resources/config_data/dataReno-Repo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nriosa\Desktop\Sanity\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nriosa\Desktop\sinIva\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1F51B0E-949A-4958-AE75-B8CF74D50C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D500B93-0078-4541-8368-5FCF78F32E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0588BB08-9742-4EC3-AC6D-1791C2B6E4F1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>URL CRM</t>
   </si>
@@ -61,13 +61,22 @@
   </si>
   <si>
     <t>Tigo.2022*</t>
+  </si>
+  <si>
+    <t>883333340718342</t>
+  </si>
+  <si>
+    <t>491453906</t>
+  </si>
+  <si>
+    <t>3043209863</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +98,12 @@
       <color rgb="FF297BDE"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,12 +127,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -433,27 +450,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC50DE46-2B7C-48D8-8E3D-CE5DBF16E4D5}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -469,14 +486,25 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16.5">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -484,5 +512,6 @@
     <hyperlink ref="A2" r:id="rId1" xr:uid="{BAB4C613-1EEE-41C8-B164-853D9C350AD1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reno-repo se actualizan clases para generar id
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/dataReno-Repo.xlsx
+++ b/src/test/resources/config_data/dataReno-Repo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nriosa\Desktop\sinIva\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D500B93-0078-4541-8368-5FCF78F32E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5423C3EC-0943-497C-93E4-2B81BFE10864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0588BB08-9742-4EC3-AC6D-1791C2B6E4F1}"/>
   </bookViews>
@@ -63,13 +63,13 @@
     <t>Tigo.2022*</t>
   </si>
   <si>
-    <t>883333340718342</t>
-  </si>
-  <si>
     <t>491453906</t>
   </si>
   <si>
-    <t>3043209863</t>
+    <t>3046010569</t>
+  </si>
+  <si>
+    <t>732111193280551</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -498,13 +498,13 @@
     </row>
     <row r="4" spans="1:3" ht="16.5">
       <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agregan las clases para el pago de equipo y ejecucion masiva
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/dataReno-Repo.xlsx
+++ b/src/test/resources/config_data/dataReno-Repo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nriosa\Desktop\sinIva\src\test\resources\config_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RenoRepo\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5423C3EC-0943-497C-93E4-2B81BFE10864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99C70A8-622C-4C3A-A3B2-4E6C94993410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0588BB08-9742-4EC3-AC6D-1791C2B6E4F1}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="18775" windowHeight="10067" xr2:uid="{0588BB08-9742-4EC3-AC6D-1791C2B6E4F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>URL CRM</t>
   </si>
@@ -63,20 +63,29 @@
     <t>Tigo.2022*</t>
   </si>
   <si>
+    <t>3045981670</t>
+  </si>
+  <si>
+    <t>3043209863</t>
+  </si>
+  <si>
+    <t>309991475</t>
+  </si>
+  <si>
     <t>491453906</t>
   </si>
   <si>
-    <t>3046010569</t>
-  </si>
-  <si>
-    <t>732111193280551</t>
+    <t>883337854391834</t>
+  </si>
+  <si>
+    <t>883338543183426</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +111,23 @@
     <font>
       <sz val="11"/>
       <color rgb="FF242424"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -127,7 +153,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -135,6 +161,8 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -450,17 +478,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC50DE46-2B7C-48D8-8E3D-CE5DBF16E4D5}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -496,18 +524,65 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:3" ht="14.95">
+      <c r="A4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.65">
+      <c r="A5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.65">
+      <c r="A6" s="5"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" ht="15.65">
+      <c r="A7" s="5"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" ht="15.65">
+      <c r="A8" s="5"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.65">
+      <c r="A9" s="5"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" ht="15.65">
+      <c r="A10" s="5"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.65">
+      <c r="A11" s="5"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" ht="15.65">
+      <c r="A12" s="5"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{BAB4C613-1EEE-41C8-B164-853D9C350AD1}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
se agrega ciclo para las lineas
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/dataReno-Repo.xlsx
+++ b/src/test/resources/config_data/dataReno-Repo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RenoRepo\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99C70A8-622C-4C3A-A3B2-4E6C94993410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5D4D4C-60C9-4B59-804D-1CD73E680109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="18775" windowHeight="10067" xr2:uid="{0588BB08-9742-4EC3-AC6D-1791C2B6E4F1}"/>
   </bookViews>
@@ -63,22 +63,22 @@
     <t>Tigo.2022*</t>
   </si>
   <si>
-    <t>3045981670</t>
-  </si>
-  <si>
-    <t>3043209863</t>
-  </si>
-  <si>
-    <t>309991475</t>
-  </si>
-  <si>
-    <t>491453906</t>
-  </si>
-  <si>
-    <t>883337854391834</t>
-  </si>
-  <si>
-    <t>883338543183426</t>
+    <t>3046010569</t>
+  </si>
+  <si>
+    <t>3046010523</t>
+  </si>
+  <si>
+    <t>163908584</t>
+  </si>
+  <si>
+    <t>270670616</t>
+  </si>
+  <si>
+    <t>883337485691834</t>
+  </si>
+  <si>
+    <t>883339511718342</t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3"/>
@@ -526,7 +526,7 @@
     </row>
     <row r="4" spans="1:3" ht="14.95">
       <c r="A4" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>9</v>
@@ -535,14 +535,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.65">
+    <row r="5" spans="1:3" ht="14.95">
       <c r="A5" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>